<commit_message>
fix bug of timeline issue
</commit_message>
<xml_diff>
--- a/batch/tasks_setting.xlsx
+++ b/batch/tasks_setting.xlsx
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=eZDmDn6Iq9Y</t>
+          <t>https://www.youtube.com/watch?v=0O2Rq4HJBxw</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -477,14 +477,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Done</t>
+          <t>Error: Summarizing and translating - Error in step 'Summarizing and translating': [red]❌ Expressiveness translation of block 80 failed after 3 retries. Please check `output/gpt_log/error.json` for more details.[/red]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=wyuZzLfDhD8</t>
+          <t>https://www.youtube.com/watch?v=Qw4l1w0rkjs</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -505,7 +505,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=0O2Rq4HJBxw&amp;list=PL30C13C91CFFEFEA6&amp;index=2</t>
+          <t>https://www.youtube.com/watch?v=MGyygiXMzRk</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -517,7 +517,11 @@
       <c r="D4" t="n">
         <v>1</v>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>